<commit_message>
remove some demo data
</commit_message>
<xml_diff>
--- a/resources/dummy_data.xlsx
+++ b/resources/dummy_data.xlsx
@@ -109,7 +109,7 @@
     <t xml:space="preserve">CC BY 4.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Fry</t>
+    <t xml:space="preserve">Some long value</t>
   </si>
   <si>
     <t xml:space="preserve">Leela</t>
@@ -340,7 +340,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -474,7 +474,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="d.banks@sussex.ac.uk"/>
+    <hyperlink ref="F2" r:id="rId1" display="This is a test image, please contact d.banks@sussex.ac.uk with any questions"/>
     <hyperlink ref="G2" r:id="rId2" display="http://www.solasistim.net/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add rest of custom fields that were left out
</commit_message>
<xml_diff>
--- a/resources/dummy_data.xlsx
+++ b/resources/dummy_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">Title </t>
   </si>
@@ -112,6 +112,9 @@
     <t xml:space="preserve">CC BY 4.0</t>
   </si>
   <si>
+    <t xml:space="preserve">A test creator</t>
+  </si>
+  <si>
     <t xml:space="preserve">Some long value</t>
   </si>
   <si>
@@ -122,6 +125,18 @@
   </si>
   <si>
     <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some test relation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A test string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another test one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Something unrelated</t>
   </si>
   <si>
     <t xml:space="preserve">eye.jpg</t>
@@ -345,8 +360,8 @@
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V3" activeCellId="0" sqref="V3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -448,34 +463,44 @@
       <c r="I2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="K2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L2" s="4" t="n">
         <v>2018</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="T2" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifying dummy data to use a real date format
</commit_message>
<xml_diff>
--- a/resources/dummy_data.xlsx
+++ b/resources/dummy_data.xlsx
@@ -164,8 +164,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -260,7 +261,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -286,6 +287,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,13 +378,13 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="14.5"/>
   </cols>
   <sheetData>
@@ -489,8 +494,8 @@
       <c r="K2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="4" t="n">
-        <v>2018</v>
+      <c r="L2" s="7" t="n">
+        <v>43185</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>34</v>
@@ -498,13 +503,13 @@
       <c r="N2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="8" t="s">
         <v>36</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="R2" s="4" t="s">

</xml_diff>